<commit_message>
Modify computation codes for Rio Grande demand and slight file name change
</commit_message>
<xml_diff>
--- a/Streamflow_Generation/consumptive.xlsx
+++ b/Streamflow_Generation/consumptive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyungmi1\Documents\Code\project-westernwaternetwork\Streamflow_Generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6466F627-FD01-42AA-915A-3D6F1685CBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24FD6CE-C418-4A47-B487-1FA1F60FA443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{91C0396D-DF00-9F4F-9744-9ABABC1C2C0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{91C0396D-DF00-9F4F-9744-9ABABC1C2C0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2884,8 +2884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE19C92E-C21C-DA48-AC64-49808EC8D5D1}">
   <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F241"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="H220" sqref="H220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>